<commit_message>
ag: cambios en los valores
</commit_message>
<xml_diff>
--- a/02_Bases de Datos 2025/MAATE/2025_05_13/recopilacion_Retenciones.xlsx
+++ b/02_Bases de Datos 2025/MAATE/2025_05_13/recopilacion_Retenciones.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Disco_F\!!Personal\Mio\1_WCS 2024\wcs\02_Bases de Datos 2025\MAATE\2025_05_13\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MAG\personal\consultorías\wcs\02_Bases de Datos 2025\MAATE\2025_05_13\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Recopilacion" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -8966,9 +8966,6 @@
     <t>nombre_comun</t>
   </si>
   <si>
-    <t>estado_especimen</t>
-  </si>
-  <si>
     <t>nro_total</t>
   </si>
   <si>
@@ -9024,6 +9021,9 @@
   </si>
   <si>
     <t>sin_nombre</t>
+  </si>
+  <si>
+    <t>elemento_retenido</t>
   </si>
 </sst>
 </file>
@@ -10339,43 +10339,41 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -10399,6 +10397,33 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -10414,19 +10439,10 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -10438,22 +10454,6 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -10796,9 +10796,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM691"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -10810,22 +10810,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="15">
-      <c r="A1" s="246" t="s">
+      <c r="A1" s="247" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="246"/>
-      <c r="C1" s="246"/>
-      <c r="D1" s="246"/>
+      <c r="B1" s="247"/>
+      <c r="C1" s="247"/>
+      <c r="D1" s="247"/>
       <c r="E1" s="248" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="249"/>
-      <c r="G1" s="247" t="s">
+      <c r="G1" s="244" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="247"/>
-      <c r="I1" s="247"/>
-      <c r="J1" s="247"/>
+      <c r="H1" s="244"/>
+      <c r="I1" s="244"/>
+      <c r="J1" s="244"/>
       <c r="K1" s="252" t="s">
         <v>3</v>
       </c>
@@ -10833,168 +10833,168 @@
       <c r="M1" s="253"/>
       <c r="N1" s="253"/>
       <c r="O1" s="254"/>
-      <c r="P1" s="255" t="s">
+      <c r="P1" s="264" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="256"/>
-      <c r="R1" s="256"/>
-      <c r="S1" s="256"/>
-      <c r="T1" s="256"/>
-      <c r="U1" s="256"/>
-      <c r="V1" s="256"/>
-      <c r="W1" s="256"/>
-      <c r="X1" s="256"/>
-      <c r="Y1" s="256"/>
-      <c r="Z1" s="256"/>
-      <c r="AA1" s="256"/>
-      <c r="AB1" s="256"/>
-      <c r="AC1" s="256"/>
-      <c r="AD1" s="256"/>
-      <c r="AE1" s="257" t="s">
+      <c r="Q1" s="265"/>
+      <c r="R1" s="265"/>
+      <c r="S1" s="265"/>
+      <c r="T1" s="265"/>
+      <c r="U1" s="265"/>
+      <c r="V1" s="265"/>
+      <c r="W1" s="265"/>
+      <c r="X1" s="265"/>
+      <c r="Y1" s="265"/>
+      <c r="Z1" s="265"/>
+      <c r="AA1" s="265"/>
+      <c r="AB1" s="265"/>
+      <c r="AC1" s="265"/>
+      <c r="AD1" s="265"/>
+      <c r="AE1" s="266" t="s">
         <v>5</v>
       </c>
-      <c r="AF1" s="258"/>
-      <c r="AG1" s="258"/>
-      <c r="AH1" s="259"/>
-      <c r="AI1" s="240" t="s">
+      <c r="AF1" s="267"/>
+      <c r="AG1" s="267"/>
+      <c r="AH1" s="268"/>
+      <c r="AI1" s="261" t="s">
         <v>6</v>
       </c>
-      <c r="AJ1" s="241"/>
-      <c r="AK1" s="241"/>
-      <c r="AL1" s="242"/>
+      <c r="AJ1" s="262"/>
+      <c r="AK1" s="262"/>
+      <c r="AL1" s="263"/>
     </row>
     <row r="2" spans="1:39" ht="15">
-      <c r="A2" s="243" t="s">
+      <c r="A2" s="255" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="244" t="s">
+      <c r="B2" s="256" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="246" t="s">
+      <c r="C2" s="247" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="246" t="s">
+      <c r="D2" s="247" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="250"/>
       <c r="F2" s="251"/>
-      <c r="G2" s="247" t="s">
+      <c r="G2" s="244" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="247" t="s">
+      <c r="H2" s="244" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="247" t="s">
+      <c r="I2" s="244" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="247" t="s">
+      <c r="J2" s="244" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="235" t="s">
+      <c r="K2" s="245" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="235" t="s">
+      <c r="L2" s="245" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="235" t="s">
+      <c r="M2" s="245" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="237" t="s">
+      <c r="N2" s="258" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="237"/>
-      <c r="P2" s="238" t="s">
+      <c r="O2" s="258"/>
+      <c r="P2" s="259" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="238" t="s">
+      <c r="Q2" s="259" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="238" t="s">
+      <c r="R2" s="259" t="s">
         <v>20</v>
       </c>
-      <c r="S2" s="238" t="s">
+      <c r="S2" s="259" t="s">
         <v>21</v>
       </c>
-      <c r="T2" s="261" t="s">
+      <c r="T2" s="269" t="s">
         <v>15</v>
       </c>
-      <c r="U2" s="238" t="s">
+      <c r="U2" s="259" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="238" t="s">
+      <c r="V2" s="259" t="s">
         <v>23</v>
       </c>
-      <c r="W2" s="263" t="s">
+      <c r="W2" s="237" t="s">
         <v>24</v>
       </c>
-      <c r="X2" s="265" t="s">
+      <c r="X2" s="271" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="266"/>
-      <c r="Z2" s="267"/>
-      <c r="AA2" s="263" t="s">
+      <c r="Y2" s="272"/>
+      <c r="Z2" s="273"/>
+      <c r="AA2" s="237" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="268" t="s">
+      <c r="AB2" s="239" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" s="269"/>
-      <c r="AD2" s="270"/>
-      <c r="AE2" s="260" t="s">
+      <c r="AC2" s="240"/>
+      <c r="AD2" s="241"/>
+      <c r="AE2" s="242" t="s">
         <v>28</v>
       </c>
-      <c r="AF2" s="260" t="s">
+      <c r="AF2" s="242" t="s">
         <v>29</v>
       </c>
-      <c r="AG2" s="271" t="s">
+      <c r="AG2" s="243" t="s">
         <v>30</v>
       </c>
-      <c r="AH2" s="271" t="s">
+      <c r="AH2" s="243" t="s">
         <v>31</v>
       </c>
-      <c r="AI2" s="272" t="s">
+      <c r="AI2" s="236" t="s">
         <v>32</v>
       </c>
-      <c r="AJ2" s="272" t="s">
+      <c r="AJ2" s="236" t="s">
         <v>33</v>
       </c>
-      <c r="AK2" s="272"/>
-      <c r="AL2" s="272" t="s">
+      <c r="AK2" s="236"/>
+      <c r="AL2" s="236" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:39" ht="30">
-      <c r="A3" s="243"/>
-      <c r="B3" s="245"/>
-      <c r="C3" s="246"/>
-      <c r="D3" s="246"/>
+      <c r="A3" s="255"/>
+      <c r="B3" s="257"/>
+      <c r="C3" s="247"/>
+      <c r="D3" s="247"/>
       <c r="E3" s="3" t="s">
         <v>35</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="247"/>
-      <c r="H3" s="247"/>
-      <c r="I3" s="247"/>
-      <c r="J3" s="247"/>
-      <c r="K3" s="236"/>
-      <c r="L3" s="236"/>
-      <c r="M3" s="236"/>
+      <c r="G3" s="244"/>
+      <c r="H3" s="244"/>
+      <c r="I3" s="244"/>
+      <c r="J3" s="244"/>
+      <c r="K3" s="246"/>
+      <c r="L3" s="246"/>
+      <c r="M3" s="246"/>
       <c r="N3" s="1" t="s">
         <v>37</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="P3" s="239"/>
-      <c r="Q3" s="239"/>
-      <c r="R3" s="239"/>
-      <c r="S3" s="239"/>
-      <c r="T3" s="262"/>
-      <c r="U3" s="239"/>
-      <c r="V3" s="239"/>
-      <c r="W3" s="264"/>
+      <c r="P3" s="260"/>
+      <c r="Q3" s="260"/>
+      <c r="R3" s="260"/>
+      <c r="S3" s="260"/>
+      <c r="T3" s="270"/>
+      <c r="U3" s="260"/>
+      <c r="V3" s="260"/>
+      <c r="W3" s="238"/>
       <c r="X3" s="4" t="s">
         <v>39</v>
       </c>
@@ -11004,7 +11004,7 @@
       <c r="Z3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AA3" s="264"/>
+      <c r="AA3" s="238"/>
       <c r="AB3" s="5" t="s">
         <v>38</v>
       </c>
@@ -11014,18 +11014,18 @@
       <c r="AD3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AE3" s="260"/>
-      <c r="AF3" s="260"/>
-      <c r="AG3" s="271"/>
-      <c r="AH3" s="271"/>
-      <c r="AI3" s="272"/>
+      <c r="AE3" s="242"/>
+      <c r="AF3" s="242"/>
+      <c r="AG3" s="243"/>
+      <c r="AH3" s="243"/>
+      <c r="AI3" s="236"/>
       <c r="AJ3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="AL3" s="272"/>
+      <c r="AL3" s="236"/>
     </row>
     <row r="4" spans="1:39" ht="42.75">
       <c r="A4" s="6" t="s">
@@ -11086,64 +11086,64 @@
         <v>2962</v>
       </c>
       <c r="T4" s="13" t="s">
+        <v>2982</v>
+      </c>
+      <c r="U4" s="15" t="s">
         <v>2963</v>
       </c>
-      <c r="U4" s="15" t="s">
+      <c r="V4" s="16" t="s">
         <v>2964</v>
       </c>
-      <c r="V4" s="16" t="s">
+      <c r="W4" s="17" t="s">
         <v>2965</v>
       </c>
-      <c r="W4" s="17" t="s">
+      <c r="X4" s="18" t="s">
         <v>2966</v>
       </c>
-      <c r="X4" s="18" t="s">
+      <c r="Y4" s="18" t="s">
         <v>2967</v>
       </c>
-      <c r="Y4" s="18" t="s">
+      <c r="Z4" s="18" t="s">
         <v>2968</v>
       </c>
-      <c r="Z4" s="18" t="s">
+      <c r="AA4" s="17" t="s">
         <v>2969</v>
       </c>
-      <c r="AA4" s="17" t="s">
+      <c r="AB4" s="19" t="s">
         <v>2970</v>
       </c>
-      <c r="AB4" s="19" t="s">
+      <c r="AC4" s="20" t="s">
         <v>2971</v>
       </c>
-      <c r="AC4" s="20" t="s">
+      <c r="AD4" s="20" t="s">
         <v>2972</v>
       </c>
-      <c r="AD4" s="20" t="s">
+      <c r="AE4" s="21" t="s">
         <v>2973</v>
       </c>
-      <c r="AE4" s="21" t="s">
+      <c r="AF4" s="21" t="s">
         <v>2974</v>
       </c>
-      <c r="AF4" s="21" t="s">
+      <c r="AG4" s="21" t="s">
         <v>2975</v>
       </c>
-      <c r="AG4" s="21" t="s">
+      <c r="AH4" s="22" t="s">
         <v>2976</v>
       </c>
-      <c r="AH4" s="22" t="s">
+      <c r="AI4" s="23" t="s">
         <v>2977</v>
       </c>
-      <c r="AI4" s="23" t="s">
+      <c r="AJ4" s="23" t="s">
         <v>2978</v>
       </c>
-      <c r="AJ4" s="23" t="s">
+      <c r="AK4" s="23" t="s">
         <v>2979</v>
       </c>
-      <c r="AK4" s="23" t="s">
+      <c r="AL4" s="24" t="s">
         <v>2980</v>
       </c>
-      <c r="AL4" s="24" t="s">
+      <c r="AM4" s="235" t="s">
         <v>2981</v>
-      </c>
-      <c r="AM4" s="273" t="s">
-        <v>2982</v>
       </c>
     </row>
     <row r="5" spans="1:39" ht="199.5">
@@ -70586,14 +70586,19 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AJ2:AK2"/>
-    <mergeCell ref="AL2:AL3"/>
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="AB2:AD2"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AH2:AH3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="AI1:AL1"/>
+    <mergeCell ref="P1:AD1"/>
+    <mergeCell ref="AE1:AH1"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="W2:W3"/>
+    <mergeCell ref="X2:Z2"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
@@ -70610,19 +70615,14 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="AI1:AL1"/>
-    <mergeCell ref="P1:AD1"/>
-    <mergeCell ref="AE1:AH1"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="X2:Z2"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="AJ2:AK2"/>
+    <mergeCell ref="AL2:AL3"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="AB2:AD2"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="AH2:AH3"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <dataValidations count="9">

</xml_diff>